<commit_message>
AddNoteToCase works both on IE and Chrome
</commit_message>
<xml_diff>
--- a/USDFramework/TC_AddNoteToCase/Main.rvl.xlsx
+++ b/USDFramework/TC_AddNoteToCase/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="105">
   <si>
     <t>Flow</t>
   </si>
@@ -295,6 +295,39 @@
   </si>
   <si>
     <t>ConfirmNoteDelete</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>LastNote</t>
+  </si>
+  <si>
+    <t>SeleniumHighlight</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>USDSelectWindow</t>
+  </si>
+  <si>
+    <t>urlOrTitleOrIndex</t>
+  </si>
+  <si>
+    <t>case</t>
   </si>
 </sst>
 </file>
@@ -315,7 +348,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="235">
+  <borders count="246">
     <border>
       <left/>
       <right/>
@@ -557,11 +590,22 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -797,6 +841,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="232" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="234" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="235" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="236" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="238" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="239" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="240" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="241" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="242" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="243" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="244" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,7 +861,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H54"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="true"/>
@@ -1122,7 +1177,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="212"/>
+      <c r="A18" s="235"/>
       <c r="B18" t="s">
         <v>30</v>
       </c>
@@ -1137,7 +1192,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="213"/>
+      <c r="A19" s="236"/>
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -1152,7 +1207,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="214"/>
+      <c r="A20" s="237"/>
       <c r="B20" t="s">
         <v>30</v>
       </c>
@@ -1167,98 +1222,90 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="221"/>
+      <c r="A21" s="238"/>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="219"/>
-      <c r="B22" t="s">
+      <c r="A22" s="240"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="241"/>
+      <c r="B23" t="s">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="221"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="219"/>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
         <v>40</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>77</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E25" t="s">
         <v>78</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F25" t="s">
         <v>79</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G25" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="229"/>
-      <c r="B23" t="s">
+    <row r="26">
+      <c r="A26" s="229"/>
+      <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>81</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" t="s">
         <v>43</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="230"/>
-      <c r="B24" t="s">
+    <row r="27">
+      <c r="A27" s="230"/>
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E27" t="s">
         <v>83</v>
-      </c>
-      <c r="F24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="220"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="207" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="231"/>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" t="s">
-        <v>42</v>
       </c>
       <c r="F27" t="s">
         <v>43</v>
@@ -1268,136 +1315,118 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="217"/>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" t="s">
-        <v>75</v>
-      </c>
+      <c r="A28" s="220"/>
     </row>
     <row r="29">
-      <c r="A29" s="226"/>
+      <c r="A29" s="207" t="s">
+        <v>7</v>
+      </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="227"/>
+      <c r="A30" s="231"/>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G30" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="209" t="s">
-        <v>7</v>
-      </c>
+      <c r="A31" s="217"/>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="G31" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="232"/>
+      <c r="A32" s="226"/>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="F32" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="233"/>
+      <c r="A33" s="227"/>
       <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="G33" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="234" t="s">
+      <c r="A34" s="209" t="s">
         <v>7</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
         <v>64</v>
@@ -1413,147 +1442,233 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="210" t="s">
-        <v>7</v>
-      </c>
+      <c r="A35" s="232"/>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="239"/>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="233"/>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="234" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="210" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
         <v>67</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D39" t="s">
         <v>64</v>
       </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="194"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="81"/>
-      <c r="B37" s="82" t="s">
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="194"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="81"/>
+      <c r="B41" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="83" t="s">
+      <c r="C41" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="84" t="s">
+      <c r="D41" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="87" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="88"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="97"/>
-      <c r="B38" s="98"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="100"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="102"/>
-      <c r="G38" s="103"/>
-      <c r="H38" s="104"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="105"/>
-      <c r="B39" s="106"/>
-      <c r="C39" s="107"/>
-      <c r="D39" s="108"/>
-      <c r="E39" s="109"/>
-      <c r="F39" s="110"/>
-      <c r="G39" s="111"/>
-      <c r="H39" s="112"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="113"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="115"/>
-      <c r="D40" s="116"/>
-      <c r="E40" s="117"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="120"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="121"/>
-      <c r="B41" s="122"/>
-      <c r="C41" s="123"/>
-      <c r="D41" s="124"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="127"/>
-      <c r="H41" s="128"/>
+      <c r="E41" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="88"/>
     </row>
     <row r="42">
-      <c r="A42" s="129"/>
-      <c r="B42" s="130"/>
-      <c r="C42" s="131"/>
-      <c r="D42" s="132"/>
-      <c r="E42" s="133"/>
-      <c r="F42" s="134"/>
-      <c r="G42" s="135"/>
-      <c r="H42" s="136"/>
+      <c r="A42" s="97"/>
+      <c r="B42" s="98"/>
+      <c r="C42" s="99"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="101"/>
+      <c r="F42" s="102"/>
+      <c r="G42" s="103"/>
+      <c r="H42" s="104"/>
     </row>
     <row r="43">
-      <c r="A43" s="137"/>
-      <c r="B43" s="138"/>
-      <c r="C43" s="139"/>
-      <c r="D43" s="140"/>
-      <c r="E43" s="141"/>
-      <c r="F43" s="142"/>
-      <c r="G43" s="143"/>
-      <c r="H43" s="144"/>
+      <c r="A43" s="105"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="107"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="109"/>
+      <c r="F43" s="110"/>
+      <c r="G43" s="111"/>
+      <c r="H43" s="112"/>
     </row>
     <row r="44">
-      <c r="A44" s="145"/>
-      <c r="B44" s="146"/>
-      <c r="C44" s="147"/>
-      <c r="D44" s="148"/>
-      <c r="E44" s="149"/>
-      <c r="F44" s="150"/>
-      <c r="G44" s="151"/>
-      <c r="H44" s="152"/>
+      <c r="A44" s="113"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="117"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="119"/>
+      <c r="H44" s="120"/>
     </row>
     <row r="45">
-      <c r="A45" s="153"/>
-      <c r="B45" s="154"/>
-      <c r="C45" s="155"/>
-      <c r="D45" s="156"/>
-      <c r="E45" s="157"/>
-      <c r="F45" s="158"/>
-      <c r="G45" s="159"/>
-      <c r="H45" s="160"/>
+      <c r="A45" s="121"/>
+      <c r="B45" s="122"/>
+      <c r="C45" s="123"/>
+      <c r="D45" s="124"/>
+      <c r="E45" s="125"/>
+      <c r="F45" s="126"/>
+      <c r="G45" s="127"/>
+      <c r="H45" s="128"/>
     </row>
     <row r="46">
-      <c r="A46" s="197"/>
+      <c r="A46" s="129"/>
+      <c r="B46" s="130"/>
+      <c r="C46" s="131"/>
+      <c r="D46" s="132"/>
+      <c r="E46" s="133"/>
+      <c r="F46" s="134"/>
+      <c r="G46" s="135"/>
+      <c r="H46" s="136"/>
     </row>
     <row r="47">
-      <c r="A47" s="198"/>
+      <c r="A47" s="137"/>
+      <c r="B47" s="138"/>
+      <c r="C47" s="139"/>
+      <c r="D47" s="140"/>
+      <c r="E47" s="141"/>
+      <c r="F47" s="142"/>
+      <c r="G47" s="143"/>
+      <c r="H47" s="144"/>
     </row>
     <row r="48">
-      <c r="A48" s="199"/>
+      <c r="A48" s="145"/>
+      <c r="B48" s="146"/>
+      <c r="C48" s="147"/>
+      <c r="D48" s="148"/>
+      <c r="E48" s="149"/>
+      <c r="F48" s="150"/>
+      <c r="G48" s="151"/>
+      <c r="H48" s="152"/>
     </row>
     <row r="49">
-      <c r="A49" s="200"/>
+      <c r="A49" s="153"/>
+      <c r="B49" s="154"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="156"/>
+      <c r="E49" s="157"/>
+      <c r="F49" s="158"/>
+      <c r="G49" s="159"/>
+      <c r="H49" s="160"/>
     </row>
     <row r="50">
-      <c r="A50" s="201"/>
+      <c r="A50" s="197"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="198"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="199"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="200"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="201"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
Updated to work with the latest Dynamics 365 build
</commit_message>
<xml_diff>
--- a/USDFramework/TC_AddNoteToCase/Main.rvl.xlsx
+++ b/USDFramework/TC_AddNoteToCase/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="114">
   <si>
     <t>Flow</t>
   </si>
@@ -331,6 +331,30 @@
   </si>
   <si>
     <t>ExpanderToggle</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t>SelectWindow</t>
+  </si>
+  <si>
+    <t>SetRichText</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>CAS-01215-N0Y1T2</t>
+  </si>
+  <si>
+    <t>Contact details requested</t>
+  </si>
+  <si>
+    <t>30000</t>
   </si>
 </sst>
 </file>
@@ -351,7 +375,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="248">
+  <borders count="252">
     <border>
       <left/>
       <right/>
@@ -606,11 +630,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -859,6 +887,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="246" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="247" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="248" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="250" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="251" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,10 +1127,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="E13" s="37" t="s">
         <v>7</v>
@@ -1134,7 +1166,7 @@
         <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16">
@@ -1180,7 +1212,7 @@
         <v>28</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
@@ -1244,7 +1276,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="240"/>
+      <c r="A22" s="251"/>
     </row>
     <row r="23">
       <c r="A23" s="241"/>
@@ -1252,10 +1284,10 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
         <v>103</v>
@@ -1421,10 +1453,10 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="E34" t="s">
         <v>87</v>
@@ -1437,7 +1469,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="227"/>
+      <c r="A35" s="249"/>
       <c r="B35" t="s">
         <v>30</v>
       </c>
@@ -1592,10 +1624,10 @@
         <v>3</v>
       </c>
       <c r="C43" s="83" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="D43" s="84" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="E43" s="85" t="s">
         <v>7</v>

</xml_diff>